<commit_message>
Add new screenshots and example database
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="log" sheetId="1" state="visible" r:id="rId2"/>
@@ -294,13 +294,13 @@
   </sheetPr>
   <dimension ref="A1:C459"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.484375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.46875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.91"/>
@@ -4350,10 +4350,10 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.484375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.46875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.91"/>
   </cols>
@@ -5094,15 +5094,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.53"/>
   </cols>
@@ -5215,7 +5215,7 @@
         <v>80</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>180</v>
@@ -5224,17 +5224,283 @@
         <v>21</v>
       </c>
       <c r="F6" s="5" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>81</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>181</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>82</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>182</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F8" s="5" t="n">
         <v>110</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>44249</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>83</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>183</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>44250</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>84</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>184</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>44251</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>170</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
+        <v>44252</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>79</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>160</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>121</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>175</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>176</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>81</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>177</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>82</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>178</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>83</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>179</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="n">
+        <v>44258</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>84</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>170</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="n">
+        <v>44259</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>160</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>